<commit_message>
* timelog * user interaction box * working on rubics cube scene
</commit_message>
<xml_diff>
--- a/doc/timelog/b.xlsx
+++ b/doc/timelog/b.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="2355" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="2805" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>upgraded to Leap SDK 2.0, read docs about new skeletal tracking, started with new domain model</t>
+  </si>
+  <si>
+    <t>physics scene refactoring, rubics cube scene</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,12 +630,21 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="2">
+        <v>41790</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.20833333333333334</v>
+      </c>
       <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333343E-2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -800,7 +812,7 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D31" s="3">
         <f>SUM(D2:D30)</f>
-        <v>0.88541666666666674</v>
+        <v>0.96875000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>